<commit_message>
gujrat state files done
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nagasudhir\Documents\Python Projects\mis\wrldc_mis_state_files_ingestion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dheer\Desktop\wrldc\wrldc_mis_state_files_ingestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B11628-6ECE-45A4-AA7C-B7C7F6B21A8B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA272D7-5659-46F0-9793-4C1C5EADBBB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,9 +35,6 @@
     <t>folder_location</t>
   </si>
   <si>
-    <t>\\10.2.100.63\g$\ETL\03_SCADA\OperationalData</t>
-  </si>
-  <si>
     <t>gujarat</t>
   </si>
   <si>
@@ -315,6 +312,9 @@
   </si>
   <si>
     <t>{{0}}*0.1</t>
+  </si>
+  <si>
+    <t>C:\Users\dheer\Desktop\wrldc\wrldc_mis_state_files_ingestion\stateFiles</t>
   </si>
 </sst>
 </file>
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -667,13 +667,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -681,36 +681,36 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{61A03ABC-49B9-4D2B-A4AB-3F4F83C9519A}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{03D9E04C-71AE-4B29-9419-441D86750EE8}"/>
+    <hyperlink ref="B2" r:id="rId1" display="\\10.2.100.63\g$\ETL\03_SCADA\OperationalData" xr:uid="{61A03ABC-49B9-4D2B-A4AB-3F4F83C9519A}"/>
+    <hyperlink ref="B3" r:id="rId2" display="\\10.2.100.63\g$\ETL\03_SCADA\OperationalData" xr:uid="{03D9E04C-71AE-4B29-9419-441D86750EE8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -720,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E411F2E-D996-44C6-8254-A1BF33A8F867}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -737,903 +737,903 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" t="s">
         <v>90</v>
       </c>
-      <c r="B1" t="s">
-        <v>91</v>
-      </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
       <c r="F1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H22" s="2"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H24" s="2"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B38" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E38" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E41" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E42" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B43" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B44" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B45" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B47" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E48" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E49" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B51" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C51" t="s">
+        <v>91</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1657,394 +1657,394 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
goa & mp done
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dheer\Desktop\wrldc\wrldc_mis_state_files_ingestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA272D7-5659-46F0-9793-4C1C5EADBBB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5043D8F8-CE55-416E-9EDA-188695AC6656}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="files_info" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="97">
   <si>
     <t>date_format</t>
   </si>
@@ -290,9 +290,6 @@
     <t>aggregation_strategy</t>
   </si>
   <si>
-    <t>Z8,Z9,Z10,Z11</t>
-  </si>
-  <si>
     <t>goa</t>
   </si>
   <si>
@@ -305,9 +302,6 @@
     <t>demand_met_mu</t>
   </si>
   <si>
-    <t>A1</t>
-  </si>
-  <si>
     <t>equation</t>
   </si>
   <si>
@@ -315,6 +309,15 @@
   </si>
   <si>
     <t>C:\Users\dheer\Desktop\wrldc\wrldc_mis_state_files_ingestion\stateFiles</t>
+  </si>
+  <si>
+    <t>AD8,AD9,AD10,AD11</t>
+  </si>
+  <si>
+    <t>GOA_{{dt}}_uploaded.xlsx</t>
+  </si>
+  <si>
+    <t>E41</t>
   </si>
 </sst>
 </file>
@@ -651,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -667,7 +670,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -684,7 +687,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -698,12 +701,26 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -720,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E411F2E-D996-44C6-8254-A1BF33A8F867}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -737,10 +754,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" t="s">
         <v>89</v>
-      </c>
-      <c r="B1" t="s">
-        <v>90</v>
       </c>
       <c r="C1" t="s">
         <v>8</v>
@@ -755,7 +772,7 @@
         <v>86</v>
       </c>
       <c r="G1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -1600,10 +1617,10 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C50" t="s">
         <v>58</v>
@@ -1612,7 +1629,7 @@
         <v>62</v>
       </c>
       <c r="E50" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
@@ -1623,17 +1640,17 @@
         <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>